<commit_message>
ultimos cambios solera Atlas
</commit_message>
<xml_diff>
--- a/Excels/Siniestros.xlsx
+++ b/Excels/Siniestros.xlsx
@@ -17,106 +17,106 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
-    <t>fechaSeguimiento</t>
-  </si>
-  <si>
-    <t>fechaTermino</t>
-  </si>
-  <si>
-    <t>idRegistro</t>
-  </si>
-  <si>
-    <t>numSiniestro</t>
-  </si>
-  <si>
-    <t>poliza</t>
-  </si>
-  <si>
-    <t>afectado</t>
-  </si>
-  <si>
-    <t>tipoDeCaso</t>
-  </si>
-  <si>
-    <t>cobertura</t>
-  </si>
-  <si>
-    <t>fechaSiniestro</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>ciudad</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>ubicacionTaller</t>
-  </si>
-  <si>
-    <t>financiado</t>
-  </si>
-  <si>
-    <t>regimenFiscal</t>
-  </si>
-  <si>
-    <t>estatusCliente</t>
-  </si>
-  <si>
-    <t>comentariosCliente</t>
-  </si>
-  <si>
-    <t>fechaCarga</t>
-  </si>
-  <si>
-    <t>fechaDecreto</t>
-  </si>
-  <si>
-    <t>usuarioCarga</t>
-  </si>
-  <si>
-    <t>estatusSeguimientoSin</t>
-  </si>
-  <si>
-    <t>usuarioAsignadoSin</t>
-  </si>
-  <si>
-    <t>fechaAsignacion</t>
-  </si>
-  <si>
-    <t>marca</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
-    <t>modelo</t>
-  </si>
-  <si>
-    <t>numSerie</t>
-  </si>
-  <si>
-    <t>valorIndemnizacion</t>
-  </si>
-  <si>
-    <t>valorComercial</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> placas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estacionProceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estatusOperativo</t>
-  </si>
-  <si>
-    <t>subEstatusProceso</t>
-  </si>
-  <si>
-    <t>usuarioSeguimiento</t>
+    <t>FECHA SEGUIMIENTO</t>
+  </si>
+  <si>
+    <t>FECHATERMINO</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>SINIESTRO</t>
+  </si>
+  <si>
+    <t>POLIZA</t>
+  </si>
+  <si>
+    <t>AFECTADO</t>
+  </si>
+  <si>
+    <t>TIPO DE CASO</t>
+  </si>
+  <si>
+    <t>COBERTURA</t>
+  </si>
+  <si>
+    <t>FECHA SINIESTRO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CIUDAD</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>UBICACION TALLER</t>
+  </si>
+  <si>
+    <t>FINANCIADO</t>
+  </si>
+  <si>
+    <t>REGIMEN FISCAL</t>
+  </si>
+  <si>
+    <t>ESTATUS CLIENTE</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>FECHA CARGA</t>
+  </si>
+  <si>
+    <t>FECHA DECRETO</t>
+  </si>
+  <si>
+    <t>USUARIO DE CARGA</t>
+  </si>
+  <si>
+    <t>ESTATUS SEGUIMIENTO</t>
+  </si>
+  <si>
+    <t>USUARIO ASIGNADO</t>
+  </si>
+  <si>
+    <t>FECHA ASIGNACION</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>MODELO</t>
+  </si>
+  <si>
+    <t>NUMERO SERIE</t>
+  </si>
+  <si>
+    <t>VALOR INDEMNIZACION</t>
+  </si>
+  <si>
+    <t>VALOR COMERCIAL</t>
+  </si>
+  <si>
+    <t>PLACAS</t>
+  </si>
+  <si>
+    <t>ESTACION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ESTATUS</t>
+  </si>
+  <si>
+    <t>SUB ESTATUS</t>
+  </si>
+  <si>
+    <t>USUARIO EN SEGUIMIENTO</t>
   </si>
   <si>
     <t>2022-12-21 11:51:30</t>
@@ -524,7 +524,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -708,27 +708,27 @@
       <c r="Y2" t="s">
         <v>51</v>
       </c>
-      <c r="AA2">
+      <c r="Z2">
         <v>2003</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AA2" t="s">
         <v>52</v>
       </c>
+      <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
-      <c r="AE2"/>
+      <c r="AE2" t="s">
+        <v>53</v>
+      </c>
       <c r="AF2" t="s">
         <v>53</v>
       </c>
       <c r="AG2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH2" t="s">
         <v>54</v>
       </c>
-      <c r="AI2"/>
+      <c r="AH2"/>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:34">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -800,31 +800,31 @@
       <c r="Y3" t="s">
         <v>51</v>
       </c>
-      <c r="AA3">
+      <c r="Z3">
         <v>2003</v>
       </c>
+      <c r="AA3" t="s">
+        <v>52</v>
+      </c>
       <c r="AB3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC3" t="s">
         <v>56</v>
       </c>
-      <c r="AD3">
+      <c r="AC3">
         <v>3</v>
       </c>
-      <c r="AE3"/>
+      <c r="AD3"/>
+      <c r="AE3" t="s">
+        <v>53</v>
+      </c>
       <c r="AF3" t="s">
         <v>53</v>
       </c>
       <c r="AG3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH3" t="s">
         <v>54</v>
       </c>
-      <c r="AI3"/>
+      <c r="AH3"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -896,29 +896,29 @@
       <c r="Y4" t="s">
         <v>51</v>
       </c>
-      <c r="AA4">
+      <c r="Z4">
         <v>2003</v>
       </c>
+      <c r="AA4" t="s">
+        <v>52</v>
+      </c>
       <c r="AB4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC4" t="s">
         <v>56</v>
       </c>
-      <c r="AD4">
+      <c r="AC4">
         <v>3</v>
       </c>
-      <c r="AE4"/>
+      <c r="AD4"/>
+      <c r="AE4" t="s">
+        <v>53</v>
+      </c>
       <c r="AF4" t="s">
         <v>53</v>
       </c>
       <c r="AG4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH4" t="s">
         <v>54</v>
       </c>
-      <c r="AI4"/>
+      <c r="AH4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>